<commit_message>
Update recurrent-only bar plot.
</commit_message>
<xml_diff>
--- a/recurrent_only_scripts/v11_v12_more_less_recurrence/chart.xlsx
+++ b/recurrent_only_scripts/v11_v12_more_less_recurrence/chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markp\Repos\18847-rTNN\mark_test_records\v11_v12_more_less_recurrence\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markb\Source\Repos\18847-rTNN\recurrent_only_scripts\v11_v12_more_less_recurrence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD2B222-6ED5-48F0-AA33-0F8B2BA80AC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF7949D-CFB0-4976-82C4-710C2C0F50BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19575" yWindow="3540" windowWidth="18855" windowHeight="15885" xr2:uid="{A423B565-34D5-47B8-A939-1DAEE50B2D02}"/>
+    <workbookView xWindow="2066" yWindow="1131" windowWidth="18583" windowHeight="12566" xr2:uid="{A423B565-34D5-47B8-A939-1DAEE50B2D02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Stronger Recurrent Weights</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t>Baseline, Sparser &amp; Stronger</t>
+  </si>
+  <si>
+    <t>Baseline, (90% Sparse)</t>
+  </si>
+  <si>
+    <t>Dual Buffers, 2x max weight</t>
+  </si>
+  <si>
+    <t>60% Sparse</t>
+  </si>
+  <si>
+    <t>98% Sp, 2x max weight</t>
+  </si>
+  <si>
+    <t>90% Sp, 2x max weight</t>
   </si>
 </sst>
 </file>
@@ -175,7 +190,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> in Recurrence for Architecture 1</a:t>
+              <a:t> on Recurrent-Only Architecture</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -222,7 +237,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Sheet1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -243,26 +258,26 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$H$1</c:f>
+              <c:f>Sheet1!$B$2:$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Baseline, 90% Sparse</c:v>
+                  <c:v>Baseline, (90% Sparse)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Baseline, Sparser &amp; Stronger</c:v>
+                  <c:v>98% Sp, 2x max weight</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Stronger Recurrent Weights</c:v>
+                  <c:v>90% Sp, 2x max weight</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>More Recurrent Weights</c:v>
+                  <c:v>60% Sparse</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Dual Buffers</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Dual Buffers, Sparser &amp; Stronger</c:v>
+                  <c:v>Dual Buffers, 2x max weight</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>No Recurrence</c:v>
@@ -272,7 +287,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$H$2</c:f>
+              <c:f>Sheet1!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -412,7 +427,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Accuracy</a:t>
+                  <a:t>Accuracy on Seq. MNIST</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -528,7 +543,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1081,15 +1096,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>217714</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>125186</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157842</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1414,16 +1429,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB328CC-6570-4D1F-AFFA-5D3CB9E155A1}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:8" ht="58.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1446,29 +1460,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" ht="58.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
         <v>21.32</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="1">
         <v>17.12</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>17.920000000000002</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E3" s="1">
         <v>14.21</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F3" s="1">
         <v>22.52</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G3" s="1">
         <v>20.420000000000002</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H3" s="1">
         <v>20.02</v>
       </c>
     </row>

</xml_diff>